<commit_message>
MAJOR REFACTORING AND CHANGES
. multiple changes, test data modification, and class creations to
upgrade the NEWUI Certification path
. pom.xml major change to fetch new SHAFT_Engine versions from a Maven
server
. removed lib folder
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification_newUI/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -44,61 +44,55 @@
     <t xml:space="preserve">URL_login_login</t>
   </si>
   <si>
-    <t xml:space="preserve">new/login</t>
+    <t xml:space="preserve">#/login</t>
   </si>
   <si>
     <t xml:space="preserve">URL_content</t>
   </si>
   <si>
-    <t xml:space="preserve">new/catalog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL_content_allContent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#/all-content</t>
+    <t xml:space="preserve">#/catalog</t>
   </si>
   <si>
     <t xml:space="preserve">URL_security_groups</t>
   </si>
   <si>
-    <t xml:space="preserve">#/security/groups</t>
+    <t xml:space="preserve">#/~/security/groups</t>
   </si>
   <si>
     <t xml:space="preserve">URL_security_users</t>
   </si>
   <si>
-    <t xml:space="preserve">#/security/users</t>
+    <t xml:space="preserve">#/~/security/users</t>
   </si>
   <si>
     <t xml:space="preserve">URL_data_dataSources</t>
   </si>
   <si>
-    <t xml:space="preserve">#/datasources/datasource</t>
+    <t xml:space="preserve">#/~/datasources/datasource</t>
   </si>
   <si>
     <t xml:space="preserve">URL_data_dataFiles</t>
   </si>
   <si>
-    <t xml:space="preserve">#/datasources/dataFiles</t>
+    <t xml:space="preserve">#/~/datasources/dataFiles</t>
   </si>
   <si>
     <t xml:space="preserve">URL_schemas_schemaList</t>
   </si>
   <si>
-    <t xml:space="preserve">#/schemas/schema-list</t>
+    <t xml:space="preserve">#/~/schemas/schema-list</t>
   </si>
   <si>
     <t xml:space="preserve">URL_scheduler_schemas</t>
   </si>
   <si>
-    <t xml:space="preserve">#/schedulers/scheduler-schemas</t>
+    <t xml:space="preserve">#/~/schedulers/scheduler-schemas</t>
   </si>
   <si>
     <t xml:space="preserve">URL_scheduler_dashboards</t>
   </si>
   <si>
-    <t xml:space="preserve">#/schedulers/scheduler-dashboards</t>
+    <t xml:space="preserve">#/~/schedulers/scheduler-dashboards</t>
   </si>
   <si>
     <t xml:space="preserve">User Credentials</t>
@@ -536,10 +530,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z49"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -909,66 +903,66 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
@@ -1007,7 +1001,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1035,130 +1029,130 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
@@ -1193,76 +1187,78 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
+      <c r="C22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1290,10 +1286,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>47</v>
@@ -1326,11 +1322,11 @@
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>49</v>
+      <c r="B25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1358,13 +1354,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>30</v>
+      <c r="C26" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1391,68 +1387,66 @@
       <c r="Z26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
@@ -1551,76 +1545,78 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1647,74 +1643,72 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1869,82 +1863,88 @@
       <c r="Z41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
-      <c r="V42" s="4"/>
-      <c r="W42" s="4"/>
-      <c r="X42" s="4"/>
-      <c r="Y42" s="4"/>
-      <c r="Z42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
+      <c r="C43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -1969,78 +1969,72 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
-      <c r="X45" s="4"/>
-      <c r="Y45" s="4"/>
-      <c r="Z45" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C47" s="4"/>
@@ -2068,38 +2062,7 @@
       <c r="Y47" s="4"/>
       <c r="Z47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-      <c r="X48" s="4"/>
-      <c r="Y48" s="4"/>
-      <c r="Z48" s="4"/>
-    </row>
+    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3052,22 +3015,22 @@
     <row r="998" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A45:C45"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B48" r:id="rId1" display="automation_robot@incorta.com"/>
+    <hyperlink ref="B47" r:id="rId1" display="automation_robot@incorta.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3100,7 +3063,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -3130,7 +3093,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3160,7 +3123,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3190,7 +3153,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -3220,7 +3183,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>

</xml_diff>